<commit_message>
TA errors fixed plus change in the goal
</commit_message>
<xml_diff>
--- a/AD-EYE/TA/Configurations/GoalConfig.xlsx
+++ b/AD-EYE/TA/Configurations/GoalConfig.xlsx
@@ -153,17 +153,16 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.58984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="8.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -179,7 +178,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>255.29</v>
+        <v>132</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -187,7 +186,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="0" t="n">
-        <v>-514.31</v>
+        <v>-314</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -203,7 +202,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="0" t="n">
-        <v>0</v>
+        <v>0.34</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -211,7 +210,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="0" t="n">
-        <v>0</v>
+        <v>0.62</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -219,7 +218,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="0" t="n">
-        <v>0.481</v>
+        <v>0.62</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -227,7 +226,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="0" t="n">
-        <v>-0.877</v>
+        <v>0.34</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
.xosc experiment A and TAOrder.csv without path issues
</commit_message>
<xml_diff>
--- a/AD-EYE/TA/Configurations/GoalConfig.xlsx
+++ b/AD-EYE/TA/Configurations/GoalConfig.xlsx
@@ -153,10 +153,10 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.58984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.39"/>
@@ -178,7 +178,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>132</v>
+        <v>154</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -186,7 +186,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="0" t="n">
-        <v>-314</v>
+        <v>-339</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>